<commit_message>
feat: implement comprehensive requirements management with CRUD operations, real-time updates, and export functionality.
</commit_message>
<xml_diff>
--- a/public/FORMATO.xlsx
+++ b/public/FORMATO.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dballon\Documents\CONTROL OBRAS\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC3593D8-F464-4866-BF24-AC1D73FA58FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69B325CA-5868-4C1E-B34D-2058C3AF97DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -977,7 +977,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="149">
+  <cellXfs count="144">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1115,9 +1115,6 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="43" fontId="10" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1128,38 +1125,14 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="10" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -1175,6 +1148,81 @@
     <xf numFmtId="0" fontId="5" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1196,69 +1244,6 @@
     <xf numFmtId="0" fontId="5" fillId="3" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1274,12 +1259,6 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -1295,101 +1274,107 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -3038,8 +3023,8 @@
   </sheetPr>
   <dimension ref="A1:H63"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" zoomScale="25" zoomScaleNormal="100" zoomScaleSheetLayoutView="25" workbookViewId="0">
-      <selection activeCell="L51" sqref="L51"/>
+    <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" topLeftCell="A5" zoomScale="70" zoomScaleNormal="100" zoomScaleSheetLayoutView="70" workbookViewId="0">
+      <selection activeCell="E17" sqref="E17:E45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3052,13 +3037,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="87"/>
-      <c r="B1" s="93" t="s">
+      <c r="A1" s="72"/>
+      <c r="B1" s="81" t="s">
         <v>19</v>
       </c>
-      <c r="C1" s="94"/>
-      <c r="D1" s="94"/>
-      <c r="E1" s="95"/>
+      <c r="C1" s="82"/>
+      <c r="D1" s="82"/>
+      <c r="E1" s="83"/>
       <c r="F1" s="29" t="s">
         <v>23</v>
       </c>
@@ -3068,11 +3053,11 @@
       <c r="H1" s="2"/>
     </row>
     <row r="2" spans="1:8" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="88"/>
-      <c r="B2" s="96"/>
-      <c r="C2" s="97"/>
-      <c r="D2" s="97"/>
-      <c r="E2" s="98"/>
+      <c r="A2" s="73"/>
+      <c r="B2" s="84"/>
+      <c r="C2" s="85"/>
+      <c r="D2" s="85"/>
+      <c r="E2" s="86"/>
       <c r="F2" s="30" t="s">
         <v>15</v>
       </c>
@@ -3082,13 +3067,13 @@
       <c r="H2" s="2"/>
     </row>
     <row r="3" spans="1:8" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="88"/>
-      <c r="B3" s="99" t="s">
+      <c r="A3" s="73"/>
+      <c r="B3" s="87" t="s">
         <v>18</v>
       </c>
-      <c r="C3" s="100"/>
-      <c r="D3" s="100"/>
-      <c r="E3" s="101"/>
+      <c r="C3" s="88"/>
+      <c r="D3" s="88"/>
+      <c r="E3" s="89"/>
       <c r="F3" s="30" t="s">
         <v>24</v>
       </c>
@@ -3098,11 +3083,11 @@
       <c r="H3" s="2"/>
     </row>
     <row r="4" spans="1:8" s="1" customFormat="1" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="89"/>
-      <c r="B4" s="102"/>
-      <c r="C4" s="103"/>
-      <c r="D4" s="103"/>
-      <c r="E4" s="104"/>
+      <c r="A4" s="74"/>
+      <c r="B4" s="90"/>
+      <c r="C4" s="91"/>
+      <c r="D4" s="91"/>
+      <c r="E4" s="92"/>
       <c r="F4" s="31" t="s">
         <v>25</v>
       </c>
@@ -3112,92 +3097,92 @@
       <c r="H4" s="2"/>
     </row>
     <row r="5" spans="1:8" s="4" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="75" t="s">
+      <c r="A5" s="66" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="90" t="s">
+      <c r="B5" s="75" t="s">
         <v>38</v>
       </c>
-      <c r="C5" s="91"/>
-      <c r="D5" s="91"/>
-      <c r="E5" s="91"/>
-      <c r="F5" s="91"/>
-      <c r="G5" s="92"/>
+      <c r="C5" s="76"/>
+      <c r="D5" s="76"/>
+      <c r="E5" s="76"/>
+      <c r="F5" s="76"/>
+      <c r="G5" s="77"/>
     </row>
     <row r="6" spans="1:8" s="4" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="72" t="s">
+      <c r="A6" s="63" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="84"/>
-      <c r="C6" s="85"/>
-      <c r="D6" s="85"/>
-      <c r="E6" s="85"/>
-      <c r="F6" s="85"/>
-      <c r="G6" s="86"/>
+      <c r="B6" s="78"/>
+      <c r="C6" s="79"/>
+      <c r="D6" s="79"/>
+      <c r="E6" s="79"/>
+      <c r="F6" s="79"/>
+      <c r="G6" s="80"/>
     </row>
     <row r="7" spans="1:8" s="4" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="72" t="s">
+      <c r="A7" s="63" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="84" t="s">
+      <c r="B7" s="78" t="s">
         <v>39</v>
       </c>
-      <c r="C7" s="85"/>
-      <c r="D7" s="85"/>
-      <c r="E7" s="85"/>
-      <c r="F7" s="85"/>
-      <c r="G7" s="86"/>
+      <c r="C7" s="79"/>
+      <c r="D7" s="79"/>
+      <c r="E7" s="79"/>
+      <c r="F7" s="79"/>
+      <c r="G7" s="80"/>
     </row>
     <row r="8" spans="1:8" s="4" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="72" t="s">
+      <c r="A8" s="63" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="84" t="s">
+      <c r="B8" s="78" t="s">
         <v>40</v>
       </c>
-      <c r="C8" s="85"/>
-      <c r="D8" s="85"/>
-      <c r="E8" s="85"/>
-      <c r="F8" s="85"/>
-      <c r="G8" s="86"/>
+      <c r="C8" s="79"/>
+      <c r="D8" s="79"/>
+      <c r="E8" s="79"/>
+      <c r="F8" s="79"/>
+      <c r="G8" s="80"/>
     </row>
     <row r="9" spans="1:8" s="4" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="72" t="s">
+      <c r="A9" s="63" t="s">
         <v>9</v>
       </c>
-      <c r="B9" s="84" t="s">
+      <c r="B9" s="78" t="s">
         <v>41</v>
       </c>
-      <c r="C9" s="85"/>
-      <c r="D9" s="85"/>
-      <c r="E9" s="85"/>
-      <c r="F9" s="85"/>
-      <c r="G9" s="86"/>
+      <c r="C9" s="79"/>
+      <c r="D9" s="79"/>
+      <c r="E9" s="79"/>
+      <c r="F9" s="79"/>
+      <c r="G9" s="80"/>
     </row>
     <row r="10" spans="1:8" s="4" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="73" t="s">
+      <c r="A10" s="64" t="s">
         <v>26</v>
       </c>
-      <c r="B10" s="84"/>
-      <c r="C10" s="85"/>
-      <c r="D10" s="85"/>
-      <c r="E10" s="85"/>
-      <c r="F10" s="85"/>
-      <c r="G10" s="86"/>
+      <c r="B10" s="78"/>
+      <c r="C10" s="79"/>
+      <c r="D10" s="79"/>
+      <c r="E10" s="79"/>
+      <c r="F10" s="79"/>
+      <c r="G10" s="80"/>
     </row>
     <row r="11" spans="1:8" s="4" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="74" t="s">
+      <c r="A11" s="65" t="s">
         <v>15</v>
       </c>
-      <c r="B11" s="81"/>
-      <c r="C11" s="82"/>
-      <c r="D11" s="82"/>
-      <c r="E11" s="82"/>
-      <c r="F11" s="82"/>
-      <c r="G11" s="83"/>
+      <c r="B11" s="97"/>
+      <c r="C11" s="98"/>
+      <c r="D11" s="98"/>
+      <c r="E11" s="98"/>
+      <c r="F11" s="98"/>
+      <c r="G11" s="99"/>
     </row>
     <row r="12" spans="1:8" s="4" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="76" t="s">
+      <c r="A12" s="67" t="s">
         <v>20</v>
       </c>
       <c r="B12" s="34"/>
@@ -3217,15 +3202,15 @@
       <c r="G13" s="13"/>
     </row>
     <row r="14" spans="1:8" s="4" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="78" t="s">
+      <c r="A14" s="94" t="s">
         <v>21</v>
       </c>
-      <c r="B14" s="79"/>
-      <c r="C14" s="79"/>
-      <c r="D14" s="79"/>
-      <c r="E14" s="79"/>
-      <c r="F14" s="79"/>
-      <c r="G14" s="80"/>
+      <c r="B14" s="95"/>
+      <c r="C14" s="95"/>
+      <c r="D14" s="95"/>
+      <c r="E14" s="95"/>
+      <c r="F14" s="95"/>
+      <c r="G14" s="96"/>
     </row>
     <row r="15" spans="1:8" s="4" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="35"/>
@@ -3233,8 +3218,8 @@
       <c r="C15" s="36"/>
       <c r="D15" s="36"/>
       <c r="E15" s="36"/>
-      <c r="F15" s="106"/>
-      <c r="G15" s="107"/>
+      <c r="F15" s="101"/>
+      <c r="G15" s="102"/>
     </row>
     <row r="16" spans="1:8" ht="33.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="51" t="s">
@@ -3261,10 +3246,10 @@
       <c r="A17" s="17">
         <v>1</v>
       </c>
-      <c r="B17" s="67"/>
-      <c r="C17" s="59"/>
-      <c r="D17" s="58"/>
-      <c r="E17" s="60"/>
+      <c r="B17" s="60"/>
+      <c r="C17" s="58"/>
+      <c r="D17" s="57"/>
+      <c r="E17" s="59"/>
       <c r="F17" s="39"/>
       <c r="G17" s="40"/>
     </row>
@@ -3272,10 +3257,10 @@
       <c r="A18" s="17">
         <v>2</v>
       </c>
-      <c r="B18" s="67"/>
-      <c r="C18" s="59"/>
-      <c r="D18" s="58"/>
-      <c r="E18" s="60"/>
+      <c r="B18" s="60"/>
+      <c r="C18" s="58"/>
+      <c r="D18" s="57"/>
+      <c r="E18" s="59"/>
       <c r="F18" s="39"/>
       <c r="G18" s="40"/>
     </row>
@@ -3283,10 +3268,10 @@
       <c r="A19" s="17">
         <v>3</v>
       </c>
-      <c r="B19" s="71"/>
-      <c r="C19" s="64"/>
-      <c r="D19" s="65"/>
-      <c r="E19" s="39"/>
+      <c r="B19" s="62"/>
+      <c r="C19" s="58"/>
+      <c r="D19" s="57"/>
+      <c r="E19" s="59"/>
       <c r="F19" s="39"/>
       <c r="G19" s="40"/>
     </row>
@@ -3294,10 +3279,10 @@
       <c r="A20" s="17">
         <v>4</v>
       </c>
-      <c r="B20" s="71"/>
-      <c r="C20" s="64"/>
-      <c r="D20" s="58"/>
-      <c r="E20" s="39"/>
+      <c r="B20" s="62"/>
+      <c r="C20" s="58"/>
+      <c r="D20" s="57"/>
+      <c r="E20" s="59"/>
       <c r="F20" s="39"/>
       <c r="G20" s="40"/>
     </row>
@@ -3305,10 +3290,10 @@
       <c r="A21" s="17">
         <v>5</v>
       </c>
-      <c r="B21" s="71"/>
-      <c r="C21" s="64"/>
-      <c r="D21" s="65"/>
-      <c r="E21" s="39"/>
+      <c r="B21" s="62"/>
+      <c r="C21" s="58"/>
+      <c r="D21" s="57"/>
+      <c r="E21" s="59"/>
       <c r="F21" s="39"/>
       <c r="G21" s="40"/>
     </row>
@@ -3316,10 +3301,10 @@
       <c r="A22" s="17">
         <v>6</v>
       </c>
-      <c r="B22" s="71"/>
-      <c r="C22" s="64"/>
-      <c r="D22" s="65"/>
-      <c r="E22" s="39"/>
+      <c r="B22" s="62"/>
+      <c r="C22" s="58"/>
+      <c r="D22" s="57"/>
+      <c r="E22" s="59"/>
       <c r="F22" s="39"/>
       <c r="G22" s="40"/>
     </row>
@@ -3328,10 +3313,10 @@
         <f>A22+1</f>
         <v>7</v>
       </c>
-      <c r="B23" s="71"/>
-      <c r="C23" s="64"/>
-      <c r="D23" s="65"/>
-      <c r="E23" s="39"/>
+      <c r="B23" s="62"/>
+      <c r="C23" s="58"/>
+      <c r="D23" s="57"/>
+      <c r="E23" s="59"/>
       <c r="F23" s="39"/>
       <c r="G23" s="40"/>
     </row>
@@ -3340,10 +3325,10 @@
         <f t="shared" ref="A24:A45" si="0">A23+1</f>
         <v>8</v>
       </c>
-      <c r="B24" s="71"/>
-      <c r="C24" s="64"/>
-      <c r="D24" s="58"/>
-      <c r="E24" s="39"/>
+      <c r="B24" s="62"/>
+      <c r="C24" s="58"/>
+      <c r="D24" s="57"/>
+      <c r="E24" s="59"/>
       <c r="F24" s="39"/>
       <c r="G24" s="40"/>
     </row>
@@ -3352,10 +3337,10 @@
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="B25" s="71"/>
-      <c r="C25" s="64"/>
-      <c r="D25" s="58"/>
-      <c r="E25" s="39"/>
+      <c r="B25" s="62"/>
+      <c r="C25" s="58"/>
+      <c r="D25" s="57"/>
+      <c r="E25" s="59"/>
       <c r="F25" s="39"/>
       <c r="G25" s="40"/>
     </row>
@@ -3364,10 +3349,10 @@
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="B26" s="67"/>
-      <c r="C26" s="64"/>
-      <c r="D26" s="58"/>
-      <c r="E26" s="39"/>
+      <c r="B26" s="60"/>
+      <c r="C26" s="58"/>
+      <c r="D26" s="57"/>
+      <c r="E26" s="59"/>
       <c r="F26" s="39"/>
       <c r="G26" s="40"/>
     </row>
@@ -3376,10 +3361,10 @@
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
-      <c r="B27" s="67"/>
-      <c r="C27" s="64"/>
-      <c r="D27" s="58"/>
-      <c r="E27" s="39"/>
+      <c r="B27" s="60"/>
+      <c r="C27" s="58"/>
+      <c r="D27" s="57"/>
+      <c r="E27" s="59"/>
       <c r="F27" s="39"/>
       <c r="G27" s="40"/>
     </row>
@@ -3388,10 +3373,10 @@
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="B28" s="63"/>
-      <c r="C28" s="59"/>
-      <c r="D28" s="58"/>
-      <c r="E28" s="62"/>
+      <c r="B28" s="68"/>
+      <c r="C28" s="58"/>
+      <c r="D28" s="57"/>
+      <c r="E28" s="142"/>
       <c r="F28" s="39"/>
       <c r="G28" s="40"/>
     </row>
@@ -3400,10 +3385,10 @@
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
-      <c r="B29" s="70"/>
-      <c r="C29" s="59"/>
-      <c r="D29" s="58"/>
-      <c r="E29" s="62"/>
+      <c r="B29" s="62"/>
+      <c r="C29" s="58"/>
+      <c r="D29" s="57"/>
+      <c r="E29" s="142"/>
       <c r="F29" s="39"/>
       <c r="G29" s="40"/>
     </row>
@@ -3412,10 +3397,10 @@
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
-      <c r="B30" s="66"/>
-      <c r="C30" s="59"/>
-      <c r="D30" s="58"/>
-      <c r="E30" s="62"/>
+      <c r="B30" s="60"/>
+      <c r="C30" s="58"/>
+      <c r="D30" s="57"/>
+      <c r="E30" s="142"/>
       <c r="F30" s="39"/>
       <c r="G30" s="40"/>
     </row>
@@ -3424,10 +3409,10 @@
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
-      <c r="B31" s="66"/>
-      <c r="C31" s="59"/>
-      <c r="D31" s="58"/>
-      <c r="E31" s="62"/>
+      <c r="B31" s="60"/>
+      <c r="C31" s="58"/>
+      <c r="D31" s="57"/>
+      <c r="E31" s="142"/>
       <c r="F31" s="39"/>
       <c r="G31" s="40"/>
     </row>
@@ -3436,10 +3421,10 @@
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
-      <c r="B32" s="66"/>
-      <c r="C32" s="59"/>
-      <c r="D32" s="58"/>
-      <c r="E32" s="62"/>
+      <c r="B32" s="60"/>
+      <c r="C32" s="58"/>
+      <c r="D32" s="57"/>
+      <c r="E32" s="142"/>
       <c r="F32" s="39"/>
       <c r="G32" s="40"/>
     </row>
@@ -3448,10 +3433,10 @@
         <f t="shared" si="0"/>
         <v>17</v>
       </c>
-      <c r="B33" s="66"/>
-      <c r="C33" s="59"/>
-      <c r="D33" s="58"/>
-      <c r="E33" s="62"/>
+      <c r="B33" s="60"/>
+      <c r="C33" s="58"/>
+      <c r="D33" s="57"/>
+      <c r="E33" s="142"/>
       <c r="F33" s="39"/>
       <c r="G33" s="40"/>
     </row>
@@ -3460,10 +3445,10 @@
         <f t="shared" si="0"/>
         <v>18</v>
       </c>
-      <c r="B34" s="66"/>
-      <c r="C34" s="59"/>
-      <c r="D34" s="58"/>
-      <c r="E34" s="62"/>
+      <c r="B34" s="60"/>
+      <c r="C34" s="58"/>
+      <c r="D34" s="57"/>
+      <c r="E34" s="142"/>
       <c r="F34" s="39"/>
       <c r="G34" s="40"/>
     </row>
@@ -3473,9 +3458,9 @@
         <v>19</v>
       </c>
       <c r="B35" s="69"/>
-      <c r="C35" s="59"/>
-      <c r="D35" s="58"/>
-      <c r="E35" s="62"/>
+      <c r="C35" s="58"/>
+      <c r="D35" s="57"/>
+      <c r="E35" s="142"/>
       <c r="F35" s="39"/>
       <c r="G35" s="40"/>
     </row>
@@ -3485,9 +3470,9 @@
         <v>20</v>
       </c>
       <c r="B36" s="69"/>
-      <c r="C36" s="59"/>
-      <c r="D36" s="58"/>
-      <c r="E36" s="62"/>
+      <c r="C36" s="58"/>
+      <c r="D36" s="57"/>
+      <c r="E36" s="142"/>
       <c r="F36" s="39"/>
       <c r="G36" s="40"/>
     </row>
@@ -3496,10 +3481,10 @@
         <f t="shared" si="0"/>
         <v>21</v>
       </c>
-      <c r="B37" s="66"/>
-      <c r="C37" s="59"/>
-      <c r="D37" s="58"/>
-      <c r="E37" s="62"/>
+      <c r="B37" s="60"/>
+      <c r="C37" s="58"/>
+      <c r="D37" s="57"/>
+      <c r="E37" s="142"/>
       <c r="F37" s="39"/>
       <c r="G37" s="40"/>
     </row>
@@ -3508,10 +3493,10 @@
         <f t="shared" si="0"/>
         <v>22</v>
       </c>
-      <c r="B38" s="68"/>
-      <c r="C38" s="59"/>
-      <c r="D38" s="58"/>
-      <c r="E38" s="62"/>
+      <c r="B38" s="61"/>
+      <c r="C38" s="58"/>
+      <c r="D38" s="57"/>
+      <c r="E38" s="142"/>
       <c r="F38" s="39"/>
       <c r="G38" s="40"/>
     </row>
@@ -3520,10 +3505,10 @@
         <f t="shared" si="0"/>
         <v>23</v>
       </c>
-      <c r="B39" s="66"/>
-      <c r="C39" s="61"/>
-      <c r="D39" s="58"/>
-      <c r="E39" s="62"/>
+      <c r="B39" s="60"/>
+      <c r="C39" s="58"/>
+      <c r="D39" s="57"/>
+      <c r="E39" s="142"/>
       <c r="F39" s="39"/>
       <c r="G39" s="40"/>
     </row>
@@ -3532,10 +3517,10 @@
         <f t="shared" si="0"/>
         <v>24</v>
       </c>
-      <c r="B40" s="66"/>
-      <c r="C40" s="61"/>
-      <c r="D40" s="58"/>
-      <c r="E40" s="57"/>
+      <c r="B40" s="60"/>
+      <c r="C40" s="58"/>
+      <c r="D40" s="57"/>
+      <c r="E40" s="143"/>
       <c r="F40" s="39"/>
       <c r="G40" s="40"/>
     </row>
@@ -3544,10 +3529,10 @@
         <f t="shared" si="0"/>
         <v>25</v>
       </c>
-      <c r="B41" s="66"/>
-      <c r="C41" s="61"/>
-      <c r="D41" s="58"/>
-      <c r="E41" s="57"/>
+      <c r="B41" s="60"/>
+      <c r="C41" s="58"/>
+      <c r="D41" s="57"/>
+      <c r="E41" s="143"/>
       <c r="F41" s="39"/>
       <c r="G41" s="40"/>
     </row>
@@ -3556,10 +3541,10 @@
         <f t="shared" si="0"/>
         <v>26</v>
       </c>
-      <c r="B42" s="66"/>
-      <c r="C42" s="61"/>
-      <c r="D42" s="61"/>
-      <c r="E42" s="57"/>
+      <c r="B42" s="60"/>
+      <c r="C42" s="58"/>
+      <c r="D42" s="57"/>
+      <c r="E42" s="143"/>
       <c r="F42" s="39"/>
       <c r="G42" s="40"/>
     </row>
@@ -3568,10 +3553,10 @@
         <f t="shared" si="0"/>
         <v>27</v>
       </c>
-      <c r="B43" s="66"/>
-      <c r="C43" s="61"/>
-      <c r="D43" s="61"/>
-      <c r="E43" s="57"/>
+      <c r="B43" s="60"/>
+      <c r="C43" s="58"/>
+      <c r="D43" s="57"/>
+      <c r="E43" s="143"/>
       <c r="F43" s="39"/>
       <c r="G43" s="40"/>
     </row>
@@ -3580,10 +3565,10 @@
         <f t="shared" si="0"/>
         <v>28</v>
       </c>
-      <c r="B44" s="66"/>
-      <c r="C44" s="61"/>
-      <c r="D44" s="61"/>
-      <c r="E44" s="57"/>
+      <c r="B44" s="60"/>
+      <c r="C44" s="58"/>
+      <c r="D44" s="57"/>
+      <c r="E44" s="143"/>
       <c r="F44" s="39"/>
       <c r="G44" s="40"/>
     </row>
@@ -3592,18 +3577,18 @@
         <f t="shared" si="0"/>
         <v>29</v>
       </c>
-      <c r="B45" s="66"/>
-      <c r="C45" s="61"/>
-      <c r="D45" s="61"/>
-      <c r="E45" s="57"/>
+      <c r="B45" s="60"/>
+      <c r="C45" s="58"/>
+      <c r="D45" s="57"/>
+      <c r="E45" s="143"/>
       <c r="F45" s="39"/>
       <c r="G45" s="40"/>
     </row>
     <row r="46" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="115" t="s">
+      <c r="A46" s="108" t="s">
         <v>29</v>
       </c>
-      <c r="B46" s="116"/>
+      <c r="B46" s="109"/>
       <c r="C46" s="53"/>
       <c r="D46" s="45"/>
       <c r="E46" s="45"/>
@@ -3611,21 +3596,21 @@
       <c r="G46" s="46"/>
     </row>
     <row r="47" spans="1:8" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="110" t="s">
+      <c r="A47" s="70" t="s">
         <v>30</v>
       </c>
-      <c r="B47" s="111"/>
-      <c r="C47" s="112"/>
-      <c r="D47" s="112"/>
-      <c r="E47" s="112"/>
-      <c r="F47" s="112"/>
-      <c r="G47" s="113"/>
+      <c r="B47" s="71"/>
+      <c r="C47" s="105"/>
+      <c r="D47" s="105"/>
+      <c r="E47" s="105"/>
+      <c r="F47" s="105"/>
+      <c r="G47" s="106"/>
     </row>
     <row r="48" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="110" t="s">
+      <c r="A48" s="70" t="s">
         <v>32</v>
       </c>
-      <c r="B48" s="111"/>
+      <c r="B48" s="71"/>
       <c r="C48" s="44"/>
       <c r="D48" s="44"/>
       <c r="E48" s="44"/>
@@ -3634,10 +3619,10 @@
       <c r="H48" s="44"/>
     </row>
     <row r="49" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="110" t="s">
+      <c r="A49" s="70" t="s">
         <v>33</v>
       </c>
-      <c r="B49" s="111"/>
+      <c r="B49" s="71"/>
       <c r="C49" s="44"/>
       <c r="D49" s="44"/>
       <c r="E49" s="44"/>
@@ -3646,10 +3631,10 @@
       <c r="H49" s="44"/>
     </row>
     <row r="50" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="110" t="s">
+      <c r="A50" s="70" t="s">
         <v>34</v>
       </c>
-      <c r="B50" s="111"/>
+      <c r="B50" s="71"/>
       <c r="C50" s="54"/>
       <c r="D50" s="54"/>
       <c r="E50" s="54"/>
@@ -3666,33 +3651,33 @@
       <c r="G51" s="43"/>
     </row>
     <row r="52" spans="1:8" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="108" t="s">
+      <c r="A52" s="103" t="s">
         <v>22</v>
       </c>
-      <c r="B52" s="108"/>
-      <c r="C52" s="108"/>
-      <c r="D52" s="108"/>
-      <c r="E52" s="108"/>
-      <c r="F52" s="108"/>
-      <c r="G52" s="108"/>
+      <c r="B52" s="103"/>
+      <c r="C52" s="103"/>
+      <c r="D52" s="103"/>
+      <c r="E52" s="103"/>
+      <c r="F52" s="103"/>
+      <c r="G52" s="103"/>
     </row>
     <row r="53" spans="1:8" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="109"/>
-      <c r="B53" s="109"/>
-      <c r="C53" s="109"/>
-      <c r="D53" s="109"/>
-      <c r="E53" s="109"/>
-      <c r="F53" s="109"/>
-      <c r="G53" s="109"/>
+      <c r="A53" s="104"/>
+      <c r="B53" s="104"/>
+      <c r="C53" s="104"/>
+      <c r="D53" s="104"/>
+      <c r="E53" s="104"/>
+      <c r="F53" s="104"/>
+      <c r="G53" s="104"/>
     </row>
     <row r="54" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="109"/>
-      <c r="B54" s="109"/>
-      <c r="C54" s="109"/>
-      <c r="D54" s="109"/>
-      <c r="E54" s="109"/>
-      <c r="F54" s="109"/>
-      <c r="G54" s="109"/>
+      <c r="A54" s="104"/>
+      <c r="B54" s="104"/>
+      <c r="C54" s="104"/>
+      <c r="D54" s="104"/>
+      <c r="E54" s="104"/>
+      <c r="F54" s="104"/>
+      <c r="G54" s="104"/>
     </row>
     <row r="55" spans="1:8" ht="12" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="62" spans="1:8" x14ac:dyDescent="0.25">
@@ -3700,27 +3685,20 @@
       <c r="B62" s="38"/>
     </row>
     <row r="63" spans="1:8" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A63" s="114" t="s">
+      <c r="A63" s="107" t="s">
         <v>28</v>
       </c>
-      <c r="B63" s="114"/>
-      <c r="C63" s="105"/>
-      <c r="D63" s="105"/>
-      <c r="E63" s="77" t="s">
+      <c r="B63" s="107"/>
+      <c r="C63" s="100"/>
+      <c r="D63" s="100"/>
+      <c r="E63" s="93" t="s">
         <v>42</v>
       </c>
-      <c r="F63" s="77"/>
-      <c r="G63" s="77"/>
+      <c r="F63" s="93"/>
+      <c r="G63" s="93"/>
     </row>
   </sheetData>
   <mergeCells count="23">
-    <mergeCell ref="A48:B48"/>
-    <mergeCell ref="A49:B49"/>
-    <mergeCell ref="A1:A4"/>
-    <mergeCell ref="B5:G5"/>
-    <mergeCell ref="B6:G6"/>
-    <mergeCell ref="B1:E2"/>
-    <mergeCell ref="B3:E4"/>
     <mergeCell ref="E63:G63"/>
     <mergeCell ref="A14:G14"/>
     <mergeCell ref="B11:G11"/>
@@ -3737,6 +3715,13 @@
     <mergeCell ref="A63:B63"/>
     <mergeCell ref="A46:B46"/>
     <mergeCell ref="A47:B47"/>
+    <mergeCell ref="A48:B48"/>
+    <mergeCell ref="A49:B49"/>
+    <mergeCell ref="A1:A4"/>
+    <mergeCell ref="B5:G5"/>
+    <mergeCell ref="B6:G6"/>
+    <mergeCell ref="B1:E2"/>
+    <mergeCell ref="B3:E4"/>
   </mergeCells>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
   <pageMargins left="0.23622047244094491" right="0.23622047244094491" top="0.55118110236220474" bottom="0.55118110236220474" header="0.31496062992125984" footer="0.31496062992125984"/>
@@ -3767,10 +3752,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="130"/>
-      <c r="B1" s="131"/>
-      <c r="C1" s="132"/>
-      <c r="D1" s="139" t="s">
+      <c r="A1" s="114"/>
+      <c r="B1" s="115"/>
+      <c r="C1" s="116"/>
+      <c r="D1" s="123" t="s">
         <v>19</v>
       </c>
       <c r="E1" s="23" t="s">
@@ -3784,10 +3769,10 @@
       <c r="I1" s="2"/>
     </row>
     <row r="2" spans="1:9" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="133"/>
-      <c r="B2" s="134"/>
-      <c r="C2" s="135"/>
-      <c r="D2" s="140"/>
+      <c r="A2" s="117"/>
+      <c r="B2" s="118"/>
+      <c r="C2" s="119"/>
+      <c r="D2" s="124"/>
       <c r="E2" s="24" t="s">
         <v>1</v>
       </c>
@@ -3799,10 +3784,10 @@
       <c r="I2" s="3"/>
     </row>
     <row r="3" spans="1:9" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="133"/>
-      <c r="B3" s="134"/>
-      <c r="C3" s="135"/>
-      <c r="D3" s="141" t="s">
+      <c r="A3" s="117"/>
+      <c r="B3" s="118"/>
+      <c r="C3" s="119"/>
+      <c r="D3" s="125" t="s">
         <v>18</v>
       </c>
       <c r="E3" s="24" t="s">
@@ -3816,10 +3801,10 @@
       <c r="I3" s="2"/>
     </row>
     <row r="4" spans="1:9" s="1" customFormat="1" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="136"/>
-      <c r="B4" s="137"/>
-      <c r="C4" s="138"/>
-      <c r="D4" s="142"/>
+      <c r="A4" s="120"/>
+      <c r="B4" s="121"/>
+      <c r="C4" s="122"/>
+      <c r="D4" s="126"/>
       <c r="E4" s="25" t="s">
         <v>3</v>
       </c>
@@ -3831,81 +3816,81 @@
       <c r="I4" s="2"/>
     </row>
     <row r="5" spans="1:9" s="4" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="143" t="s">
+      <c r="A5" s="127" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="144"/>
-      <c r="C5" s="144"/>
-      <c r="D5" s="145"/>
-      <c r="E5" s="145"/>
-      <c r="F5" s="146"/>
+      <c r="B5" s="128"/>
+      <c r="C5" s="128"/>
+      <c r="D5" s="129"/>
+      <c r="E5" s="129"/>
+      <c r="F5" s="130"/>
     </row>
     <row r="6" spans="1:9" s="4" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="120" t="s">
+      <c r="A6" s="110" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="121"/>
-      <c r="C6" s="121"/>
-      <c r="D6" s="122"/>
-      <c r="E6" s="122"/>
-      <c r="F6" s="123"/>
+      <c r="B6" s="111"/>
+      <c r="C6" s="111"/>
+      <c r="D6" s="112"/>
+      <c r="E6" s="112"/>
+      <c r="F6" s="113"/>
     </row>
     <row r="7" spans="1:9" s="4" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="120" t="s">
+      <c r="A7" s="110" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="121"/>
-      <c r="C7" s="121"/>
-      <c r="D7" s="122"/>
-      <c r="E7" s="122"/>
-      <c r="F7" s="123"/>
+      <c r="B7" s="111"/>
+      <c r="C7" s="111"/>
+      <c r="D7" s="112"/>
+      <c r="E7" s="112"/>
+      <c r="F7" s="113"/>
     </row>
     <row r="8" spans="1:9" s="4" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="120" t="s">
+      <c r="A8" s="110" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="121"/>
-      <c r="C8" s="121"/>
-      <c r="D8" s="122"/>
-      <c r="E8" s="122"/>
-      <c r="F8" s="123"/>
+      <c r="B8" s="111"/>
+      <c r="C8" s="111"/>
+      <c r="D8" s="112"/>
+      <c r="E8" s="112"/>
+      <c r="F8" s="113"/>
     </row>
     <row r="9" spans="1:9" s="4" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="120" t="s">
+      <c r="A9" s="110" t="s">
         <v>9</v>
       </c>
-      <c r="B9" s="121"/>
-      <c r="C9" s="121"/>
-      <c r="D9" s="122"/>
-      <c r="E9" s="122"/>
-      <c r="F9" s="123"/>
+      <c r="B9" s="111"/>
+      <c r="C9" s="111"/>
+      <c r="D9" s="112"/>
+      <c r="E9" s="112"/>
+      <c r="F9" s="113"/>
     </row>
     <row r="10" spans="1:9" s="4" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="120" t="s">
+      <c r="A10" s="110" t="s">
         <v>10</v>
       </c>
-      <c r="B10" s="121"/>
-      <c r="C10" s="121"/>
-      <c r="D10" s="122"/>
-      <c r="E10" s="122"/>
-      <c r="F10" s="123"/>
+      <c r="B10" s="111"/>
+      <c r="C10" s="111"/>
+      <c r="D10" s="112"/>
+      <c r="E10" s="112"/>
+      <c r="F10" s="113"/>
     </row>
     <row r="11" spans="1:9" s="4" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="124" t="s">
+      <c r="A11" s="131" t="s">
         <v>15</v>
       </c>
-      <c r="B11" s="125"/>
-      <c r="C11" s="125"/>
-      <c r="D11" s="126"/>
-      <c r="E11" s="126"/>
-      <c r="F11" s="127"/>
+      <c r="B11" s="132"/>
+      <c r="C11" s="132"/>
+      <c r="D11" s="133"/>
+      <c r="E11" s="133"/>
+      <c r="F11" s="134"/>
     </row>
     <row r="12" spans="1:9" s="4" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="128" t="s">
+      <c r="A12" s="135" t="s">
         <v>20</v>
       </c>
-      <c r="B12" s="129"/>
-      <c r="C12" s="129"/>
+      <c r="B12" s="136"/>
+      <c r="C12" s="136"/>
       <c r="D12" s="9"/>
       <c r="E12" s="9"/>
       <c r="F12" s="10"/>
@@ -3919,24 +3904,24 @@
       <c r="F13" s="13"/>
     </row>
     <row r="14" spans="1:9" s="4" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="78" t="s">
+      <c r="A14" s="94" t="s">
         <v>21</v>
       </c>
-      <c r="B14" s="79"/>
-      <c r="C14" s="79"/>
-      <c r="D14" s="79"/>
-      <c r="E14" s="79"/>
-      <c r="F14" s="80"/>
+      <c r="B14" s="95"/>
+      <c r="C14" s="95"/>
+      <c r="D14" s="95"/>
+      <c r="E14" s="95"/>
+      <c r="F14" s="96"/>
     </row>
     <row r="15" spans="1:9" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="B15" s="119" t="s">
+      <c r="B15" s="138" t="s">
         <v>12</v>
       </c>
-      <c r="C15" s="119"/>
-      <c r="D15" s="119"/>
+      <c r="C15" s="138"/>
+      <c r="D15" s="138"/>
       <c r="E15" s="22" t="s">
         <v>13</v>
       </c>
@@ -3948,9 +3933,9 @@
       <c r="A16" s="17">
         <v>1</v>
       </c>
-      <c r="B16" s="117"/>
-      <c r="C16" s="117"/>
-      <c r="D16" s="117"/>
+      <c r="B16" s="137"/>
+      <c r="C16" s="137"/>
+      <c r="D16" s="137"/>
       <c r="E16" s="14"/>
       <c r="F16" s="18"/>
     </row>
@@ -3958,9 +3943,9 @@
       <c r="A17" s="17">
         <v>2</v>
       </c>
-      <c r="B17" s="117"/>
-      <c r="C17" s="117"/>
-      <c r="D17" s="117"/>
+      <c r="B17" s="137"/>
+      <c r="C17" s="137"/>
+      <c r="D17" s="137"/>
       <c r="E17" s="14"/>
       <c r="F17" s="18"/>
     </row>
@@ -3968,9 +3953,9 @@
       <c r="A18" s="17">
         <v>3</v>
       </c>
-      <c r="B18" s="117"/>
-      <c r="C18" s="117"/>
-      <c r="D18" s="117"/>
+      <c r="B18" s="137"/>
+      <c r="C18" s="137"/>
+      <c r="D18" s="137"/>
       <c r="E18" s="14"/>
       <c r="F18" s="18"/>
     </row>
@@ -3978,9 +3963,9 @@
       <c r="A19" s="17">
         <v>4</v>
       </c>
-      <c r="B19" s="117"/>
-      <c r="C19" s="117"/>
-      <c r="D19" s="117"/>
+      <c r="B19" s="137"/>
+      <c r="C19" s="137"/>
+      <c r="D19" s="137"/>
       <c r="E19" s="14"/>
       <c r="F19" s="18"/>
     </row>
@@ -3988,9 +3973,9 @@
       <c r="A20" s="17">
         <v>5</v>
       </c>
-      <c r="B20" s="117"/>
-      <c r="C20" s="117"/>
-      <c r="D20" s="117"/>
+      <c r="B20" s="137"/>
+      <c r="C20" s="137"/>
+      <c r="D20" s="137"/>
       <c r="E20" s="14"/>
       <c r="F20" s="18"/>
     </row>
@@ -3998,9 +3983,9 @@
       <c r="A21" s="17">
         <v>6</v>
       </c>
-      <c r="B21" s="117"/>
-      <c r="C21" s="117"/>
-      <c r="D21" s="117"/>
+      <c r="B21" s="137"/>
+      <c r="C21" s="137"/>
+      <c r="D21" s="137"/>
       <c r="E21" s="14"/>
       <c r="F21" s="18"/>
     </row>
@@ -4008,9 +3993,9 @@
       <c r="A22" s="17">
         <v>7</v>
       </c>
-      <c r="B22" s="117"/>
-      <c r="C22" s="117"/>
-      <c r="D22" s="117"/>
+      <c r="B22" s="137"/>
+      <c r="C22" s="137"/>
+      <c r="D22" s="137"/>
       <c r="E22" s="14"/>
       <c r="F22" s="18"/>
     </row>
@@ -4018,9 +4003,9 @@
       <c r="A23" s="17">
         <v>8</v>
       </c>
-      <c r="B23" s="117"/>
-      <c r="C23" s="117"/>
-      <c r="D23" s="117"/>
+      <c r="B23" s="137"/>
+      <c r="C23" s="137"/>
+      <c r="D23" s="137"/>
       <c r="E23" s="14"/>
       <c r="F23" s="18"/>
     </row>
@@ -4028,9 +4013,9 @@
       <c r="A24" s="17">
         <v>9</v>
       </c>
-      <c r="B24" s="117"/>
-      <c r="C24" s="117"/>
-      <c r="D24" s="117"/>
+      <c r="B24" s="137"/>
+      <c r="C24" s="137"/>
+      <c r="D24" s="137"/>
       <c r="E24" s="14"/>
       <c r="F24" s="18"/>
     </row>
@@ -4038,9 +4023,9 @@
       <c r="A25" s="17">
         <v>10</v>
       </c>
-      <c r="B25" s="117"/>
-      <c r="C25" s="117"/>
-      <c r="D25" s="117"/>
+      <c r="B25" s="137"/>
+      <c r="C25" s="137"/>
+      <c r="D25" s="137"/>
       <c r="E25" s="14"/>
       <c r="F25" s="18"/>
     </row>
@@ -4048,9 +4033,9 @@
       <c r="A26" s="17">
         <v>11</v>
       </c>
-      <c r="B26" s="117"/>
-      <c r="C26" s="117"/>
-      <c r="D26" s="117"/>
+      <c r="B26" s="137"/>
+      <c r="C26" s="137"/>
+      <c r="D26" s="137"/>
       <c r="E26" s="14"/>
       <c r="F26" s="18"/>
     </row>
@@ -4058,9 +4043,9 @@
       <c r="A27" s="17">
         <v>12</v>
       </c>
-      <c r="B27" s="117"/>
-      <c r="C27" s="117"/>
-      <c r="D27" s="117"/>
+      <c r="B27" s="137"/>
+      <c r="C27" s="137"/>
+      <c r="D27" s="137"/>
       <c r="E27" s="14"/>
       <c r="F27" s="18"/>
     </row>
@@ -4068,9 +4053,9 @@
       <c r="A28" s="17">
         <v>13</v>
       </c>
-      <c r="B28" s="117"/>
-      <c r="C28" s="117"/>
-      <c r="D28" s="117"/>
+      <c r="B28" s="137"/>
+      <c r="C28" s="137"/>
+      <c r="D28" s="137"/>
       <c r="E28" s="14"/>
       <c r="F28" s="18"/>
     </row>
@@ -4078,9 +4063,9 @@
       <c r="A29" s="17">
         <v>14</v>
       </c>
-      <c r="B29" s="117"/>
-      <c r="C29" s="117"/>
-      <c r="D29" s="117"/>
+      <c r="B29" s="137"/>
+      <c r="C29" s="137"/>
+      <c r="D29" s="137"/>
       <c r="E29" s="14"/>
       <c r="F29" s="18"/>
     </row>
@@ -4088,9 +4073,9 @@
       <c r="A30" s="17">
         <v>15</v>
       </c>
-      <c r="B30" s="117"/>
-      <c r="C30" s="117"/>
-      <c r="D30" s="117"/>
+      <c r="B30" s="137"/>
+      <c r="C30" s="137"/>
+      <c r="D30" s="137"/>
       <c r="E30" s="14"/>
       <c r="F30" s="18"/>
     </row>
@@ -4098,9 +4083,9 @@
       <c r="A31" s="17">
         <v>16</v>
       </c>
-      <c r="B31" s="117"/>
-      <c r="C31" s="117"/>
-      <c r="D31" s="117"/>
+      <c r="B31" s="137"/>
+      <c r="C31" s="137"/>
+      <c r="D31" s="137"/>
       <c r="E31" s="14"/>
       <c r="F31" s="18"/>
     </row>
@@ -4108,9 +4093,9 @@
       <c r="A32" s="17">
         <v>17</v>
       </c>
-      <c r="B32" s="117"/>
-      <c r="C32" s="117"/>
-      <c r="D32" s="117"/>
+      <c r="B32" s="137"/>
+      <c r="C32" s="137"/>
+      <c r="D32" s="137"/>
       <c r="E32" s="14"/>
       <c r="F32" s="18"/>
     </row>
@@ -4118,9 +4103,9 @@
       <c r="A33" s="17">
         <v>18</v>
       </c>
-      <c r="B33" s="117"/>
-      <c r="C33" s="117"/>
-      <c r="D33" s="117"/>
+      <c r="B33" s="137"/>
+      <c r="C33" s="137"/>
+      <c r="D33" s="137"/>
       <c r="E33" s="14"/>
       <c r="F33" s="18"/>
     </row>
@@ -4128,9 +4113,9 @@
       <c r="A34" s="17">
         <v>19</v>
       </c>
-      <c r="B34" s="117"/>
-      <c r="C34" s="117"/>
-      <c r="D34" s="117"/>
+      <c r="B34" s="137"/>
+      <c r="C34" s="137"/>
+      <c r="D34" s="137"/>
       <c r="E34" s="14"/>
       <c r="F34" s="18"/>
     </row>
@@ -4138,21 +4123,35 @@
       <c r="A35" s="19">
         <v>20</v>
       </c>
-      <c r="B35" s="118"/>
-      <c r="C35" s="118"/>
-      <c r="D35" s="118"/>
+      <c r="B35" s="139"/>
+      <c r="C35" s="139"/>
+      <c r="D35" s="139"/>
       <c r="E35" s="20"/>
       <c r="F35" s="21"/>
     </row>
   </sheetData>
   <mergeCells count="40">
-    <mergeCell ref="A6:C6"/>
-    <mergeCell ref="D6:F6"/>
-    <mergeCell ref="A1:C4"/>
-    <mergeCell ref="D1:D2"/>
-    <mergeCell ref="D3:D4"/>
-    <mergeCell ref="A5:C5"/>
-    <mergeCell ref="D5:F5"/>
+    <mergeCell ref="B33:D33"/>
+    <mergeCell ref="B34:D34"/>
+    <mergeCell ref="B35:D35"/>
+    <mergeCell ref="B27:D27"/>
+    <mergeCell ref="B28:D28"/>
+    <mergeCell ref="B29:D29"/>
+    <mergeCell ref="B30:D30"/>
+    <mergeCell ref="B31:D31"/>
+    <mergeCell ref="B32:D32"/>
+    <mergeCell ref="B26:D26"/>
+    <mergeCell ref="B15:D15"/>
+    <mergeCell ref="B16:D16"/>
+    <mergeCell ref="B17:D17"/>
+    <mergeCell ref="B18:D18"/>
+    <mergeCell ref="B19:D19"/>
+    <mergeCell ref="B20:D20"/>
+    <mergeCell ref="B21:D21"/>
+    <mergeCell ref="B22:D22"/>
+    <mergeCell ref="B23:D23"/>
+    <mergeCell ref="B24:D24"/>
+    <mergeCell ref="B25:D25"/>
     <mergeCell ref="A14:F14"/>
     <mergeCell ref="A7:C7"/>
     <mergeCell ref="D7:F7"/>
@@ -4165,27 +4164,13 @@
     <mergeCell ref="A11:C11"/>
     <mergeCell ref="D11:F11"/>
     <mergeCell ref="A12:C12"/>
-    <mergeCell ref="B26:D26"/>
-    <mergeCell ref="B15:D15"/>
-    <mergeCell ref="B16:D16"/>
-    <mergeCell ref="B17:D17"/>
-    <mergeCell ref="B18:D18"/>
-    <mergeCell ref="B19:D19"/>
-    <mergeCell ref="B20:D20"/>
-    <mergeCell ref="B21:D21"/>
-    <mergeCell ref="B22:D22"/>
-    <mergeCell ref="B23:D23"/>
-    <mergeCell ref="B24:D24"/>
-    <mergeCell ref="B25:D25"/>
-    <mergeCell ref="B33:D33"/>
-    <mergeCell ref="B34:D34"/>
-    <mergeCell ref="B35:D35"/>
-    <mergeCell ref="B27:D27"/>
-    <mergeCell ref="B28:D28"/>
-    <mergeCell ref="B29:D29"/>
-    <mergeCell ref="B30:D30"/>
-    <mergeCell ref="B31:D31"/>
-    <mergeCell ref="B32:D32"/>
+    <mergeCell ref="A6:C6"/>
+    <mergeCell ref="D6:F6"/>
+    <mergeCell ref="A1:C4"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="D3:D4"/>
+    <mergeCell ref="A5:C5"/>
+    <mergeCell ref="D5:F5"/>
   </mergeCells>
   <pageMargins left="0.74" right="0.46" top="0.53" bottom="0.27" header="0.31496062992125984" footer="0.18"/>
   <pageSetup paperSize="9" scale="68" orientation="portrait" r:id="rId1"/>
@@ -4215,10 +4200,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="130"/>
-      <c r="B1" s="131"/>
-      <c r="C1" s="132"/>
-      <c r="D1" s="147" t="s">
+      <c r="A1" s="114"/>
+      <c r="B1" s="115"/>
+      <c r="C1" s="116"/>
+      <c r="D1" s="140" t="s">
         <v>19</v>
       </c>
       <c r="E1" s="26" t="s">
@@ -4232,10 +4217,10 @@
       <c r="I1" s="2"/>
     </row>
     <row r="2" spans="1:9" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="133"/>
-      <c r="B2" s="134"/>
-      <c r="C2" s="135"/>
-      <c r="D2" s="148"/>
+      <c r="A2" s="117"/>
+      <c r="B2" s="118"/>
+      <c r="C2" s="119"/>
+      <c r="D2" s="141"/>
       <c r="E2" s="27" t="s">
         <v>1</v>
       </c>
@@ -4247,10 +4232,10 @@
       <c r="I2" s="3"/>
     </row>
     <row r="3" spans="1:9" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="133"/>
-      <c r="B3" s="134"/>
-      <c r="C3" s="135"/>
-      <c r="D3" s="141" t="s">
+      <c r="A3" s="117"/>
+      <c r="B3" s="118"/>
+      <c r="C3" s="119"/>
+      <c r="D3" s="125" t="s">
         <v>18</v>
       </c>
       <c r="E3" s="27" t="s">
@@ -4264,10 +4249,10 @@
       <c r="I3" s="2"/>
     </row>
     <row r="4" spans="1:9" s="1" customFormat="1" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="136"/>
-      <c r="B4" s="137"/>
-      <c r="C4" s="138"/>
-      <c r="D4" s="142"/>
+      <c r="A4" s="120"/>
+      <c r="B4" s="121"/>
+      <c r="C4" s="122"/>
+      <c r="D4" s="126"/>
       <c r="E4" s="28" t="s">
         <v>3</v>
       </c>
@@ -4279,81 +4264,81 @@
       <c r="I4" s="2"/>
     </row>
     <row r="5" spans="1:9" s="4" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="143" t="s">
+      <c r="A5" s="127" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="144"/>
-      <c r="C5" s="144"/>
-      <c r="D5" s="145"/>
-      <c r="E5" s="145"/>
-      <c r="F5" s="146"/>
+      <c r="B5" s="128"/>
+      <c r="C5" s="128"/>
+      <c r="D5" s="129"/>
+      <c r="E5" s="129"/>
+      <c r="F5" s="130"/>
     </row>
     <row r="6" spans="1:9" s="4" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="120" t="s">
+      <c r="A6" s="110" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="121"/>
-      <c r="C6" s="121"/>
-      <c r="D6" s="122"/>
-      <c r="E6" s="122"/>
-      <c r="F6" s="123"/>
+      <c r="B6" s="111"/>
+      <c r="C6" s="111"/>
+      <c r="D6" s="112"/>
+      <c r="E6" s="112"/>
+      <c r="F6" s="113"/>
     </row>
     <row r="7" spans="1:9" s="4" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="120" t="s">
+      <c r="A7" s="110" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="121"/>
-      <c r="C7" s="121"/>
-      <c r="D7" s="122"/>
-      <c r="E7" s="122"/>
-      <c r="F7" s="123"/>
+      <c r="B7" s="111"/>
+      <c r="C7" s="111"/>
+      <c r="D7" s="112"/>
+      <c r="E7" s="112"/>
+      <c r="F7" s="113"/>
     </row>
     <row r="8" spans="1:9" s="4" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="120" t="s">
+      <c r="A8" s="110" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="121"/>
-      <c r="C8" s="121"/>
-      <c r="D8" s="122"/>
-      <c r="E8" s="122"/>
-      <c r="F8" s="123"/>
+      <c r="B8" s="111"/>
+      <c r="C8" s="111"/>
+      <c r="D8" s="112"/>
+      <c r="E8" s="112"/>
+      <c r="F8" s="113"/>
     </row>
     <row r="9" spans="1:9" s="4" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="120" t="s">
+      <c r="A9" s="110" t="s">
         <v>9</v>
       </c>
-      <c r="B9" s="121"/>
-      <c r="C9" s="121"/>
-      <c r="D9" s="122"/>
-      <c r="E9" s="122"/>
-      <c r="F9" s="123"/>
+      <c r="B9" s="111"/>
+      <c r="C9" s="111"/>
+      <c r="D9" s="112"/>
+      <c r="E9" s="112"/>
+      <c r="F9" s="113"/>
     </row>
     <row r="10" spans="1:9" s="4" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="120" t="s">
+      <c r="A10" s="110" t="s">
         <v>10</v>
       </c>
-      <c r="B10" s="121"/>
-      <c r="C10" s="121"/>
-      <c r="D10" s="122"/>
-      <c r="E10" s="122"/>
-      <c r="F10" s="123"/>
+      <c r="B10" s="111"/>
+      <c r="C10" s="111"/>
+      <c r="D10" s="112"/>
+      <c r="E10" s="112"/>
+      <c r="F10" s="113"/>
     </row>
     <row r="11" spans="1:9" s="4" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="124" t="s">
+      <c r="A11" s="131" t="s">
         <v>15</v>
       </c>
-      <c r="B11" s="125"/>
-      <c r="C11" s="125"/>
-      <c r="D11" s="126"/>
-      <c r="E11" s="126"/>
-      <c r="F11" s="127"/>
+      <c r="B11" s="132"/>
+      <c r="C11" s="132"/>
+      <c r="D11" s="133"/>
+      <c r="E11" s="133"/>
+      <c r="F11" s="134"/>
     </row>
     <row r="12" spans="1:9" s="4" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="128" t="s">
+      <c r="A12" s="135" t="s">
         <v>20</v>
       </c>
-      <c r="B12" s="129"/>
-      <c r="C12" s="129"/>
+      <c r="B12" s="136"/>
+      <c r="C12" s="136"/>
       <c r="D12" s="9"/>
       <c r="E12" s="9"/>
       <c r="F12" s="10"/>
@@ -4367,24 +4352,24 @@
       <c r="F13" s="13"/>
     </row>
     <row r="14" spans="1:9" s="4" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="78" t="s">
+      <c r="A14" s="94" t="s">
         <v>21</v>
       </c>
-      <c r="B14" s="79"/>
-      <c r="C14" s="79"/>
-      <c r="D14" s="79"/>
-      <c r="E14" s="79"/>
-      <c r="F14" s="80"/>
+      <c r="B14" s="95"/>
+      <c r="C14" s="95"/>
+      <c r="D14" s="95"/>
+      <c r="E14" s="95"/>
+      <c r="F14" s="96"/>
     </row>
     <row r="15" spans="1:9" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="B15" s="119" t="s">
+      <c r="B15" s="138" t="s">
         <v>12</v>
       </c>
-      <c r="C15" s="119"/>
-      <c r="D15" s="119"/>
+      <c r="C15" s="138"/>
+      <c r="D15" s="138"/>
       <c r="E15" s="22" t="s">
         <v>13</v>
       </c>
@@ -4396,9 +4381,9 @@
       <c r="A16" s="17">
         <v>1</v>
       </c>
-      <c r="B16" s="117"/>
-      <c r="C16" s="117"/>
-      <c r="D16" s="117"/>
+      <c r="B16" s="137"/>
+      <c r="C16" s="137"/>
+      <c r="D16" s="137"/>
       <c r="E16" s="14"/>
       <c r="F16" s="18"/>
     </row>
@@ -4406,9 +4391,9 @@
       <c r="A17" s="17">
         <v>2</v>
       </c>
-      <c r="B17" s="117"/>
-      <c r="C17" s="117"/>
-      <c r="D17" s="117"/>
+      <c r="B17" s="137"/>
+      <c r="C17" s="137"/>
+      <c r="D17" s="137"/>
       <c r="E17" s="14"/>
       <c r="F17" s="18"/>
     </row>
@@ -4416,9 +4401,9 @@
       <c r="A18" s="17">
         <v>3</v>
       </c>
-      <c r="B18" s="117"/>
-      <c r="C18" s="117"/>
-      <c r="D18" s="117"/>
+      <c r="B18" s="137"/>
+      <c r="C18" s="137"/>
+      <c r="D18" s="137"/>
       <c r="E18" s="14"/>
       <c r="F18" s="18"/>
     </row>
@@ -4426,9 +4411,9 @@
       <c r="A19" s="17">
         <v>4</v>
       </c>
-      <c r="B19" s="117"/>
-      <c r="C19" s="117"/>
-      <c r="D19" s="117"/>
+      <c r="B19" s="137"/>
+      <c r="C19" s="137"/>
+      <c r="D19" s="137"/>
       <c r="E19" s="14"/>
       <c r="F19" s="18"/>
     </row>
@@ -4436,9 +4421,9 @@
       <c r="A20" s="17">
         <v>5</v>
       </c>
-      <c r="B20" s="117"/>
-      <c r="C20" s="117"/>
-      <c r="D20" s="117"/>
+      <c r="B20" s="137"/>
+      <c r="C20" s="137"/>
+      <c r="D20" s="137"/>
       <c r="E20" s="14"/>
       <c r="F20" s="18"/>
     </row>
@@ -4446,9 +4431,9 @@
       <c r="A21" s="17">
         <v>6</v>
       </c>
-      <c r="B21" s="117"/>
-      <c r="C21" s="117"/>
-      <c r="D21" s="117"/>
+      <c r="B21" s="137"/>
+      <c r="C21" s="137"/>
+      <c r="D21" s="137"/>
       <c r="E21" s="14"/>
       <c r="F21" s="18"/>
     </row>
@@ -4456,9 +4441,9 @@
       <c r="A22" s="17">
         <v>7</v>
       </c>
-      <c r="B22" s="117"/>
-      <c r="C22" s="117"/>
-      <c r="D22" s="117"/>
+      <c r="B22" s="137"/>
+      <c r="C22" s="137"/>
+      <c r="D22" s="137"/>
       <c r="E22" s="14"/>
       <c r="F22" s="18"/>
     </row>
@@ -4466,9 +4451,9 @@
       <c r="A23" s="17">
         <v>8</v>
       </c>
-      <c r="B23" s="117"/>
-      <c r="C23" s="117"/>
-      <c r="D23" s="117"/>
+      <c r="B23" s="137"/>
+      <c r="C23" s="137"/>
+      <c r="D23" s="137"/>
       <c r="E23" s="14"/>
       <c r="F23" s="18"/>
     </row>
@@ -4476,9 +4461,9 @@
       <c r="A24" s="17">
         <v>9</v>
       </c>
-      <c r="B24" s="117"/>
-      <c r="C24" s="117"/>
-      <c r="D24" s="117"/>
+      <c r="B24" s="137"/>
+      <c r="C24" s="137"/>
+      <c r="D24" s="137"/>
       <c r="E24" s="14"/>
       <c r="F24" s="18"/>
     </row>
@@ -4486,9 +4471,9 @@
       <c r="A25" s="17">
         <v>10</v>
       </c>
-      <c r="B25" s="117"/>
-      <c r="C25" s="117"/>
-      <c r="D25" s="117"/>
+      <c r="B25" s="137"/>
+      <c r="C25" s="137"/>
+      <c r="D25" s="137"/>
       <c r="E25" s="14"/>
       <c r="F25" s="18"/>
     </row>
@@ -4496,9 +4481,9 @@
       <c r="A26" s="17">
         <v>11</v>
       </c>
-      <c r="B26" s="117"/>
-      <c r="C26" s="117"/>
-      <c r="D26" s="117"/>
+      <c r="B26" s="137"/>
+      <c r="C26" s="137"/>
+      <c r="D26" s="137"/>
       <c r="E26" s="14"/>
       <c r="F26" s="18"/>
     </row>
@@ -4506,9 +4491,9 @@
       <c r="A27" s="17">
         <v>12</v>
       </c>
-      <c r="B27" s="117"/>
-      <c r="C27" s="117"/>
-      <c r="D27" s="117"/>
+      <c r="B27" s="137"/>
+      <c r="C27" s="137"/>
+      <c r="D27" s="137"/>
       <c r="E27" s="14"/>
       <c r="F27" s="18"/>
     </row>
@@ -4516,9 +4501,9 @@
       <c r="A28" s="17">
         <v>13</v>
       </c>
-      <c r="B28" s="117"/>
-      <c r="C28" s="117"/>
-      <c r="D28" s="117"/>
+      <c r="B28" s="137"/>
+      <c r="C28" s="137"/>
+      <c r="D28" s="137"/>
       <c r="E28" s="14"/>
       <c r="F28" s="18"/>
     </row>
@@ -4526,9 +4511,9 @@
       <c r="A29" s="17">
         <v>14</v>
       </c>
-      <c r="B29" s="117"/>
-      <c r="C29" s="117"/>
-      <c r="D29" s="117"/>
+      <c r="B29" s="137"/>
+      <c r="C29" s="137"/>
+      <c r="D29" s="137"/>
       <c r="E29" s="14"/>
       <c r="F29" s="18"/>
     </row>
@@ -4536,9 +4521,9 @@
       <c r="A30" s="17">
         <v>15</v>
       </c>
-      <c r="B30" s="117"/>
-      <c r="C30" s="117"/>
-      <c r="D30" s="117"/>
+      <c r="B30" s="137"/>
+      <c r="C30" s="137"/>
+      <c r="D30" s="137"/>
       <c r="E30" s="14"/>
       <c r="F30" s="18"/>
     </row>
@@ -4546,9 +4531,9 @@
       <c r="A31" s="17">
         <v>16</v>
       </c>
-      <c r="B31" s="117"/>
-      <c r="C31" s="117"/>
-      <c r="D31" s="117"/>
+      <c r="B31" s="137"/>
+      <c r="C31" s="137"/>
+      <c r="D31" s="137"/>
       <c r="E31" s="14"/>
       <c r="F31" s="18"/>
     </row>
@@ -4556,9 +4541,9 @@
       <c r="A32" s="17">
         <v>17</v>
       </c>
-      <c r="B32" s="117"/>
-      <c r="C32" s="117"/>
-      <c r="D32" s="117"/>
+      <c r="B32" s="137"/>
+      <c r="C32" s="137"/>
+      <c r="D32" s="137"/>
       <c r="E32" s="14"/>
       <c r="F32" s="18"/>
     </row>
@@ -4566,9 +4551,9 @@
       <c r="A33" s="17">
         <v>18</v>
       </c>
-      <c r="B33" s="117"/>
-      <c r="C33" s="117"/>
-      <c r="D33" s="117"/>
+      <c r="B33" s="137"/>
+      <c r="C33" s="137"/>
+      <c r="D33" s="137"/>
       <c r="E33" s="14"/>
       <c r="F33" s="18"/>
     </row>
@@ -4576,9 +4561,9 @@
       <c r="A34" s="17">
         <v>19</v>
       </c>
-      <c r="B34" s="117"/>
-      <c r="C34" s="117"/>
-      <c r="D34" s="117"/>
+      <c r="B34" s="137"/>
+      <c r="C34" s="137"/>
+      <c r="D34" s="137"/>
       <c r="E34" s="14"/>
       <c r="F34" s="18"/>
     </row>
@@ -4586,21 +4571,35 @@
       <c r="A35" s="19">
         <v>20</v>
       </c>
-      <c r="B35" s="118"/>
-      <c r="C35" s="118"/>
-      <c r="D35" s="118"/>
+      <c r="B35" s="139"/>
+      <c r="C35" s="139"/>
+      <c r="D35" s="139"/>
       <c r="E35" s="20"/>
       <c r="F35" s="21"/>
     </row>
   </sheetData>
   <mergeCells count="40">
-    <mergeCell ref="A6:C6"/>
-    <mergeCell ref="D6:F6"/>
-    <mergeCell ref="A1:C4"/>
-    <mergeCell ref="D1:D2"/>
-    <mergeCell ref="D3:D4"/>
-    <mergeCell ref="A5:C5"/>
-    <mergeCell ref="D5:F5"/>
+    <mergeCell ref="B33:D33"/>
+    <mergeCell ref="B34:D34"/>
+    <mergeCell ref="B35:D35"/>
+    <mergeCell ref="B27:D27"/>
+    <mergeCell ref="B28:D28"/>
+    <mergeCell ref="B29:D29"/>
+    <mergeCell ref="B30:D30"/>
+    <mergeCell ref="B31:D31"/>
+    <mergeCell ref="B32:D32"/>
+    <mergeCell ref="B26:D26"/>
+    <mergeCell ref="B15:D15"/>
+    <mergeCell ref="B16:D16"/>
+    <mergeCell ref="B17:D17"/>
+    <mergeCell ref="B18:D18"/>
+    <mergeCell ref="B19:D19"/>
+    <mergeCell ref="B20:D20"/>
+    <mergeCell ref="B21:D21"/>
+    <mergeCell ref="B22:D22"/>
+    <mergeCell ref="B23:D23"/>
+    <mergeCell ref="B24:D24"/>
+    <mergeCell ref="B25:D25"/>
     <mergeCell ref="A14:F14"/>
     <mergeCell ref="A7:C7"/>
     <mergeCell ref="D7:F7"/>
@@ -4613,27 +4612,13 @@
     <mergeCell ref="A11:C11"/>
     <mergeCell ref="D11:F11"/>
     <mergeCell ref="A12:C12"/>
-    <mergeCell ref="B26:D26"/>
-    <mergeCell ref="B15:D15"/>
-    <mergeCell ref="B16:D16"/>
-    <mergeCell ref="B17:D17"/>
-    <mergeCell ref="B18:D18"/>
-    <mergeCell ref="B19:D19"/>
-    <mergeCell ref="B20:D20"/>
-    <mergeCell ref="B21:D21"/>
-    <mergeCell ref="B22:D22"/>
-    <mergeCell ref="B23:D23"/>
-    <mergeCell ref="B24:D24"/>
-    <mergeCell ref="B25:D25"/>
-    <mergeCell ref="B33:D33"/>
-    <mergeCell ref="B34:D34"/>
-    <mergeCell ref="B35:D35"/>
-    <mergeCell ref="B27:D27"/>
-    <mergeCell ref="B28:D28"/>
-    <mergeCell ref="B29:D29"/>
-    <mergeCell ref="B30:D30"/>
-    <mergeCell ref="B31:D31"/>
-    <mergeCell ref="B32:D32"/>
+    <mergeCell ref="A6:C6"/>
+    <mergeCell ref="D6:F6"/>
+    <mergeCell ref="A1:C4"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="D3:D4"/>
+    <mergeCell ref="A5:C5"/>
+    <mergeCell ref="D5:F5"/>
   </mergeCells>
   <pageMargins left="0.74" right="0.46" top="0.53" bottom="0.27" header="0.31496062992125984" footer="0.18"/>
   <pageSetup paperSize="9" scale="68" orientation="portrait" r:id="rId1"/>

</xml_diff>